<commit_message>
initial database and springboot api
</commit_message>
<xml_diff>
--- a/info/table.xlsx
+++ b/info/table.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>USER</t>
   </si>
@@ -98,6 +98,12 @@
     <t>email</t>
   </si>
   <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
     <t>RECORD</t>
   </si>
   <si>
@@ -111,9 +117,6 @@
   </si>
   <si>
     <t>content</t>
-  </si>
-  <si>
-    <t>status</t>
   </si>
   <si>
     <t>boolean</t>
@@ -1310,7 +1313,7 @@
   <dimension ref="B2:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1469,7 +1472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:12">
       <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
@@ -1482,22 +1485,34 @@
       <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="K8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:12">
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2"/>
       <c r="E12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -1517,13 +1532,13 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>7</v>
@@ -1531,7 +1546,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>12</v>
@@ -1545,15 +1560,15 @@
     </row>
     <row r="16" spans="5:6">
       <c r="E16" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="5:6">
       <c r="E17" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>18</v>
@@ -1561,7 +1576,7 @@
     </row>
     <row r="18" spans="5:6">
       <c r="E18" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>18</v>

</xml_diff>